<commit_message>
Finish Lab 5 code
</commit_message>
<xml_diff>
--- a/testfiles/ExpectedResultsTable.xlsx
+++ b/testfiles/ExpectedResultsTable.xlsx
@@ -571,8 +571,8 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B20" sqref="B20"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,9 +729,7 @@
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4">
-        <v>40</v>
-      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>

</xml_diff>

<commit_message>
Finished Lab 5 with Report
</commit_message>
<xml_diff>
--- a/testfiles/ExpectedResultsTable.xlsx
+++ b/testfiles/ExpectedResultsTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ELC3338\Team8\CompOrg_Spring2018_S1_Team8\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Computer Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="53">
   <si>
     <t>Instruction 1</t>
   </si>
@@ -170,13 +170,19 @@
     <t>8A0A02CB</t>
   </si>
   <si>
-    <t>3FFFFFFFFFFFFFFFFFB</t>
-  </si>
-  <si>
     <t>‭17FFFFC9‬</t>
   </si>
   <si>
     <t xml:space="preserve">x will equal 0 </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>FFFF FFFF FFFF FFFB</t>
+  </si>
+  <si>
+    <t>FFFF FFFF FFFF FFC9</t>
   </si>
 </sst>
 </file>
@@ -262,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -276,7 +282,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -572,19 +577,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F5" sqref="F5"/>
+      <selection pane="topRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -659,34 +667,34 @@
       <c r="A3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>14000040</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="I3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -729,157 +737,175 @@
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="4">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="4">
+        <v>60</v>
+      </c>
       <c r="F5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="G5" s="4">
+        <v>8</v>
+      </c>
+      <c r="H5" s="4">
+        <v>40</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>42</v>
+      <c r="B6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>42</v>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>42</v>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>42</v>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1057,13 +1083,16 @@
         <v>42</v>
       </c>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+    </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+        <v>49</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -1082,14 +1111,14 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E19" s="10"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="15"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="16"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>

</xml_diff>

<commit_message>
Lab 6 Mostly Done
</commit_message>
<xml_diff>
--- a/testfiles/ExpectedResultsTable.xlsx
+++ b/testfiles/ExpectedResultsTable.xlsx
@@ -231,7 +231,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +274,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -364,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -397,7 +403,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,8 +690,8 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H13" sqref="H13"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,12 +1297,12 @@
         <v>15</v>
       </c>
       <c r="C22" s="24">
-        <v>0</v>
-      </c>
-      <c r="D22" s="4">
+        <v>10</v>
+      </c>
+      <c r="D22" s="24">
         <v>30</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="24">
         <v>15</v>
       </c>
       <c r="F22" s="24">
@@ -1302,7 +1311,7 @@
       <c r="G22" s="24">
         <v>0</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="25" t="s">
         <v>41</v>
       </c>
       <c r="I22" s="10" t="s">
@@ -1323,31 +1332,31 @@
         <v>41</v>
       </c>
       <c r="C23" s="24">
-        <v>10</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="D23" s="24">
+        <v>30</v>
       </c>
       <c r="E23" s="24">
+        <v>0</v>
+      </c>
+      <c r="F23" s="24">
+        <v>0</v>
+      </c>
+      <c r="G23" s="24">
+        <v>0</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="4">
+        <v>9</v>
+      </c>
+      <c r="K23" s="4">
         <v>30</v>
-      </c>
-      <c r="F23" s="24">
-        <v>30</v>
-      </c>
-      <c r="G23" s="24">
-        <v>30</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="4">
-        <v>0</v>
-      </c>
-      <c r="K23" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1357,22 +1366,22 @@
       <c r="B24" s="12">
         <v>0</v>
       </c>
-      <c r="C24" s="4">
-        <v>0</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0</v>
-      </c>
-      <c r="F24" s="4">
-        <v>0</v>
-      </c>
-      <c r="G24" s="4">
-        <v>0</v>
-      </c>
-      <c r="H24" s="4">
+      <c r="C24" s="24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="24">
+        <v>0</v>
+      </c>
+      <c r="H24" s="24">
         <v>1</v>
       </c>
       <c r="I24" s="4">

</xml_diff>

<commit_message>
Lab 9 Almost Done
</commit_message>
<xml_diff>
--- a/testfiles/ExpectedResultsTable.xlsx
+++ b/testfiles/ExpectedResultsTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
   <si>
     <t>Instruction 1</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t>000101xxxx</t>
+  </si>
+  <si>
+    <t>execute_branch_target</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>alu_result</t>
   </si>
 </sst>
 </file>
@@ -293,7 +302,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -366,11 +375,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -407,6 +469,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,9 +769,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,58 +1789,129 @@
         <v>10001010000</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>62</v>
+    <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="26">
+        <v>256</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="26">
+        <v>396</v>
+      </c>
+      <c r="F36" s="26">
+        <v>-4</v>
+      </c>
+      <c r="G36" s="26">
+        <v>52</v>
+      </c>
+      <c r="H36" s="26">
+        <v>280</v>
+      </c>
+      <c r="I36" s="26">
+        <v>-192</v>
+      </c>
+      <c r="J36" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K36" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="19">
+        <v>0</v>
+      </c>
+      <c r="C37" s="19">
+        <v>0</v>
+      </c>
+      <c r="D37" s="19">
+        <v>1</v>
+      </c>
+      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="F37" s="32">
+        <v>1</v>
+      </c>
+      <c r="G37" s="32">
+        <v>0</v>
+      </c>
+      <c r="H37" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="J37" s="19">
+        <v>0</v>
+      </c>
+      <c r="K37" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="28">
+        <v>79</v>
+      </c>
+      <c r="C38" s="28">
+        <v>30</v>
+      </c>
+      <c r="D38" s="28">
+        <v>0</v>
+      </c>
+      <c r="E38" s="28">
+        <v>111</v>
+      </c>
+      <c r="F38" s="28">
+        <v>0</v>
+      </c>
+      <c r="G38" s="28">
+        <v>20</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I38" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="J38" s="28">
+        <v>30</v>
+      </c>
+      <c r="K38" s="29">
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
       <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
-      <c r="B40" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
-      <c r="B41" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
-      <c r="B42" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="9"/>
       <c r="D42" s="9"/>
     </row>
-    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
-      <c r="B43" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -1789,20 +1940,20 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
       <c r="D48" s="9"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
+      <c r="B49" t="s">
+        <v>62</v>
+      </c>
       <c r="D49" s="9"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
       <c r="D50" s="9"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1813,26 +1964,40 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
+      <c r="B52" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="D52" s="9"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
+      <c r="B53" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="D53" s="9"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
+      <c r="B54" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
+      <c r="B55" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>